<commit_message>
change to enrollment extension to mimic existing ALR
</commit_message>
<xml_diff>
--- a/prototype/alr_ig/output/StructureDefinition-ext-enrollmentFlag.xlsx
+++ b/prototype/alr_ig/output/StructureDefinition-ext-enrollmentFlag.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="81">
   <si>
     <t>Path</t>
   </si>
@@ -206,7 +206,7 @@
     <t>Element.extension</t>
   </si>
   <si>
-    <t>period</t>
+    <t>monthNum</t>
   </si>
   <si>
     <t>An Extension</t>
@@ -243,7 +243,7 @@
     <t>Extension.extension.value[x]</t>
   </si>
   <si>
-    <t xml:space="preserve">Period
+    <t xml:space="preserve">integer
 </t>
   </si>
   <si>
@@ -261,10 +261,6 @@
   </si>
   <si>
     <t>flag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coding
-</t>
   </si>
   <si>
     <t>http://alr.cms.gov/ig/StructureDefinition/ext-enrollmentFlag</t>
@@ -430,7 +426,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="28.2734375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.1328125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="11.3359375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="12.3828125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
@@ -1812,7 +1808,7 @@
         <v>37</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="K14" t="s" s="2">
         <v>74</v>
@@ -1929,7 +1925,7 @@
       </c>
       <c r="P15" s="2"/>
       <c r="Q15" t="s" s="2">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="R15" t="s" s="2">
         <v>37</v>
@@ -2014,7 +2010,7 @@
         <v>37</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K16" t="s" s="2">
         <v>74</v>

</xml_diff>